<commit_message>
Sort based on success with translating the "other" direction
</commit_message>
<xml_diff>
--- a/pair_lists/German_groups.xlsx
+++ b/pair_lists/German_groups.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="-15" windowWidth="10815" windowHeight="10245"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="64">
   <si>
     <t>Numbers to 20</t>
   </si>
@@ -186,9 +186,6 @@
     <t>Weather</t>
   </si>
   <si>
-    <t>Essential words</t>
-  </si>
-  <si>
     <t>Miscellaneous 1</t>
   </si>
   <si>
@@ -205,6 +202,12 @@
   </si>
   <si>
     <t>People</t>
+  </si>
+  <si>
+    <t>Words from books</t>
+  </si>
+  <si>
+    <t>Verb examples</t>
   </si>
 </sst>
 </file>
@@ -543,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B68"/>
+  <dimension ref="A1:B69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,98 +623,98 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -735,7 +738,7 @@
         <v>38</v>
       </c>
       <c r="B23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -743,7 +746,7 @@
         <v>40</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -767,7 +770,7 @@
         <v>46</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -791,284 +794,284 @@
         <v>52</v>
       </c>
       <c r="B30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B31" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B32" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B33" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B34" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B35" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B36" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B37" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B38" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B39" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B40" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B41" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B42" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B43" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B44" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B45" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B46" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B47" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B48" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B49" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B50" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B51" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B52" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B53" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B54" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B55" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B56" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B57" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B58" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B59" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B60" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B61" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B62" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B63" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B64" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B65" t="s">
         <v>43</v>
@@ -1076,31 +1079,39 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B66" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B67" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68">
+        <v>98</v>
+      </c>
+      <c r="B68" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
         <v>99</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B69" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A1:B69">
-    <sortCondition ref="A1:A69"/>
+  <sortState ref="A1:B68">
+    <sortCondition ref="A1:A68"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updates to German list and groups
</commit_message>
<xml_diff>
--- a/pair_lists/German_groups.xlsx
+++ b/pair_lists/German_groups.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="66">
   <si>
     <t>Numbers to 20</t>
   </si>
@@ -204,10 +204,16 @@
     <t>People</t>
   </si>
   <si>
-    <t>Words from books</t>
-  </si>
-  <si>
     <t>Verb examples</t>
+  </si>
+  <si>
+    <t>Words from books and newspapers</t>
+  </si>
+  <si>
+    <t>Church</t>
+  </si>
+  <si>
+    <t>Miscellaneous 6</t>
   </si>
 </sst>
 </file>
@@ -546,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B69"/>
+  <dimension ref="A1:B71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,7 +752,7 @@
         <v>40</v>
       </c>
       <c r="B24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -802,316 +808,332 @@
         <v>54</v>
       </c>
       <c r="B31" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B32" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B33" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B34" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B35" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B36" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B37" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B38" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B39" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B40" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B41" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B42" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B43" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B44" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B45" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B46" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B47" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B48" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B49" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B50" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B51" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B52" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B53" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B54" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B55" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B56" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B58" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B59" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B60" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B61" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B62" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B63" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B64" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B65" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B66" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B67" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B68" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69">
+        <v>97</v>
+      </c>
+      <c r="B69" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>98</v>
+      </c>
+      <c r="B70" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71">
         <v>99</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B71" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A1:B68">
-    <sortCondition ref="A1:A68"/>
+  <sortState ref="A1:B71">
+    <sortCondition ref="A1:A71"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>